<commit_message>
Katalon Studio IVY BIMBO
</commit_message>
<xml_diff>
--- a/DDF/Phase2.1/CommonData/CommonData.xlsx
+++ b/DDF/Phase2.1/CommonData/CommonData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Bimbo Mobile\DDF\Phase2\Common_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\Bimbo Mobile-TY-02022022-1456\Bimbo Mobile-TY\DDF\Phase2.1\Common_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="500"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CommonData" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="249">
   <si>
     <t>OdometerReading</t>
   </si>
@@ -747,6 +747,30 @@
   </si>
   <si>
     <t>IVA%</t>
+  </si>
+  <si>
+    <t>02_BIM_SKU_EP_SD</t>
+  </si>
+  <si>
+    <t>03_BIM_SKU_EP_SD</t>
+  </si>
+  <si>
+    <t>04_BIM_SKU_EP</t>
+  </si>
+  <si>
+    <t>05_BIM_SKU_EP</t>
+  </si>
+  <si>
+    <t>02_BCL_SKU_EP</t>
+  </si>
+  <si>
+    <t>03_BCL_SKU_EP</t>
+  </si>
+  <si>
+    <t>04_BCL_SKU_EP</t>
+  </si>
+  <si>
+    <t>05_BCL_SKU_EP</t>
   </si>
 </sst>
 </file>
@@ -1200,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S70"/>
+  <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2369,6 +2393,46 @@
         <v>233</v>
       </c>
     </row>
+    <row r="71" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F71" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="72" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F72" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="73" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F73" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="74" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F74" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="75" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F75" s="9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="76" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F76" s="9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="77" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F77" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="78" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F78" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>